<commit_message>
Format fixes Comma-delimiter and removed all semicolon (;) and quotation marks (") index,...,index,value,,unit,source,updated at,updated by
Signed-off-by: Stian Backe <Stian.Backe@sintef.no>
</commit_message>
<xml_diff>
--- a/00_Sources/REF2020_Technology Assumptions_Energy.xlsx
+++ b/00_Sources/REF2020_Technology Assumptions_Energy.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5E86B2-851B-44BC-8249-688302E8C7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11235" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Domestic" sheetId="7" r:id="rId1"/>
@@ -1432,10 +1432,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -2371,7 +2371,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="538">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2483,10 +2483,10 @@
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2501,7 +2501,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2561,13 +2561,13 @@
     <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="12" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="12" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="12" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="12" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="17" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2588,13 +2588,13 @@
     <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="13" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="13" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="13" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="13" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="17" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2618,109 +2618,109 @@
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="26" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="26" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="26" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="26" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="26" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="26" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="26" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="26" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="26" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="26" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="26" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="26" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="15" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="15" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="15" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="15" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="15" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="15" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="15" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="15" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="15" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="15" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="15" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="15" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="14" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="14" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="14" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="14" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="14" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="14" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="14" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="14" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="14" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="14" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="14" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="14" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="22" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="22" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="22" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="22" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="22" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="22" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="22" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="22" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="22" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="22" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="22" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="22" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="22" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="22" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="22" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="22" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2729,136 +2729,136 @@
     <xf numFmtId="0" fontId="17" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="27" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="27" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="27" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="27" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="27" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="27" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="27" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="27" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="22" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="22" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="22" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="22" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="22" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="22" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="22" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="22" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="22" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="22" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="22" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="22" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="22" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="22" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="22" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="17" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="18" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="18" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="18" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="18" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="18" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="18" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="18" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="18" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="18" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="18" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="17" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="19" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="19" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="19" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="19" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="19" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="19" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="19" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="19" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="19" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="19" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="19" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="19" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="18" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="18" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="18" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="18" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="18" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="18" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="18" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="18" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="18" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="18" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="18" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="18" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2870,71 +2870,71 @@
     <xf numFmtId="0" fontId="17" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="25" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="12" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="12" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="14" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="14" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="14" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="14" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="14" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="14" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="14" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="14" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="20" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="20" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="20" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="20" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="20" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="20" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="16" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="16" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="16" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="16" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="16" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="16" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="22" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="22" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="22" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="22" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="22" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="22" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2946,13 +2946,13 @@
     <xf numFmtId="0" fontId="17" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="20" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="20" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="20" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="20" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="20" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="20" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3009,13 +3009,13 @@
     <xf numFmtId="1" fontId="17" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3030,13 +3030,13 @@
     <xf numFmtId="1" fontId="17" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="16" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="16" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="16" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="16" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="16" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3075,13 +3075,13 @@
     <xf numFmtId="1" fontId="17" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="18" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="18" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="18" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="18" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="17" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3099,40 +3099,40 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="3" fillId="20" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="20" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="20" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="20" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="21" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="21" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="21" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="21" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="20" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="20" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="20" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="20" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="20" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="20" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="12" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="12" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="12" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="12" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3153,32 +3153,32 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="19" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="19" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="7" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="5" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="32" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="32" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="32" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="32" borderId="9" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="32" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="36" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="37" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="38" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="39" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="40" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="41" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="36" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="37" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="38" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="39" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="40" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="41" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="43" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="44" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="45" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="43" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="44" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="45" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="33" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3222,19 +3222,19 @@
     <xf numFmtId="1" fontId="7" fillId="34" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="34" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="7" fillId="34" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="34" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="7" fillId="34" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="34" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="34" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="34" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="34" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="34" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3268,9 +3268,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="35" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="35" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="7" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="35" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="7" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="35" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3278,8 +3278,8 @@
     <xf numFmtId="1" fontId="7" fillId="35" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="7" fillId="35" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="7" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="35" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="35" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="7" fillId="35" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="7" fillId="35" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="7" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3299,15 +3299,15 @@
     <xf numFmtId="1" fontId="3" fillId="36" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="36" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="36" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="35" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="35" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="36" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="34" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="34" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="34" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="35" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="35" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="35" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="36" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="34" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="34" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="34" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="35" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3399,8 +3399,119 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="36" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="36" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="36" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="36" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="33" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="33" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="33" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3413,15 +3524,6 @@
     <xf numFmtId="0" fontId="5" fillId="30" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3431,114 +3533,12 @@
     <xf numFmtId="0" fontId="5" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="33" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="33" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="33" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3602,6 +3602,15 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="7" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="5" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="7" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="7" fillId="35" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3614,14 +3623,8 @@
     <xf numFmtId="0" fontId="10" fillId="30" borderId="5" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="7" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="5" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="7" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3640,9 +3643,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="25" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="25" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3979,23 +3979,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="453" t="s">
+      <c r="A1" s="490" t="s">
         <v>317</v>
       </c>
-      <c r="B1" s="454"/>
-      <c r="C1" s="454"/>
-      <c r="D1" s="454"/>
-      <c r="E1" s="454"/>
-      <c r="F1" s="454"/>
-      <c r="G1" s="454"/>
-      <c r="H1" s="454"/>
-      <c r="I1" s="454"/>
-      <c r="J1" s="454"/>
-      <c r="K1" s="454"/>
-      <c r="L1" s="454"/>
-      <c r="M1" s="454"/>
-      <c r="N1" s="454"/>
-      <c r="O1" s="454"/>
+      <c r="B1" s="491"/>
+      <c r="C1" s="491"/>
+      <c r="D1" s="491"/>
+      <c r="E1" s="491"/>
+      <c r="F1" s="491"/>
+      <c r="G1" s="491"/>
+      <c r="H1" s="491"/>
+      <c r="I1" s="491"/>
+      <c r="J1" s="491"/>
+      <c r="K1" s="491"/>
+      <c r="L1" s="491"/>
+      <c r="M1" s="491"/>
+      <c r="N1" s="491"/>
+      <c r="O1" s="491"/>
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -4017,81 +4017,81 @@
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="455" t="s">
+      <c r="A3" s="492" t="s">
         <v>189</v>
       </c>
-      <c r="B3" s="456"/>
-      <c r="C3" s="456"/>
-      <c r="D3" s="456"/>
-      <c r="E3" s="456"/>
-      <c r="F3" s="456"/>
-      <c r="G3" s="456"/>
-      <c r="H3" s="456"/>
-      <c r="I3" s="456"/>
-      <c r="J3" s="456"/>
-      <c r="K3" s="456"/>
-      <c r="L3" s="456"/>
-      <c r="M3" s="456"/>
-      <c r="N3" s="456"/>
-      <c r="O3" s="456"/>
+      <c r="B3" s="493"/>
+      <c r="C3" s="493"/>
+      <c r="D3" s="493"/>
+      <c r="E3" s="493"/>
+      <c r="F3" s="493"/>
+      <c r="G3" s="493"/>
+      <c r="H3" s="493"/>
+      <c r="I3" s="493"/>
+      <c r="J3" s="493"/>
+      <c r="K3" s="493"/>
+      <c r="L3" s="493"/>
+      <c r="M3" s="493"/>
+      <c r="N3" s="493"/>
+      <c r="O3" s="493"/>
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="457" t="s">
+      <c r="B4" s="486" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="457"/>
-      <c r="D4" s="457"/>
-      <c r="E4" s="457"/>
-      <c r="F4" s="457"/>
-      <c r="G4" s="457"/>
-      <c r="H4" s="458"/>
-      <c r="I4" s="459" t="s">
+      <c r="C4" s="486"/>
+      <c r="D4" s="486"/>
+      <c r="E4" s="486"/>
+      <c r="F4" s="486"/>
+      <c r="G4" s="486"/>
+      <c r="H4" s="487"/>
+      <c r="I4" s="485" t="s">
         <v>131</v>
       </c>
-      <c r="J4" s="457"/>
-      <c r="K4" s="457"/>
-      <c r="L4" s="457"/>
-      <c r="M4" s="457"/>
-      <c r="N4" s="457"/>
-      <c r="O4" s="458"/>
+      <c r="J4" s="486"/>
+      <c r="K4" s="486"/>
+      <c r="L4" s="486"/>
+      <c r="M4" s="486"/>
+      <c r="N4" s="486"/>
+      <c r="O4" s="487"/>
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="289"/>
-      <c r="B5" s="466" t="s">
+      <c r="B5" s="497" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="459">
+      <c r="C5" s="485">
         <v>2030</v>
       </c>
-      <c r="D5" s="457"/>
-      <c r="E5" s="458"/>
-      <c r="F5" s="459" t="s">
+      <c r="D5" s="486"/>
+      <c r="E5" s="487"/>
+      <c r="F5" s="485" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="457"/>
-      <c r="H5" s="458"/>
-      <c r="I5" s="468" t="s">
+      <c r="G5" s="486"/>
+      <c r="H5" s="487"/>
+      <c r="I5" s="488" t="s">
         <v>67</v>
       </c>
-      <c r="J5" s="459">
+      <c r="J5" s="485">
         <v>2030</v>
       </c>
-      <c r="K5" s="457"/>
-      <c r="L5" s="458"/>
-      <c r="M5" s="459" t="s">
+      <c r="K5" s="486"/>
+      <c r="L5" s="487"/>
+      <c r="M5" s="485" t="s">
         <v>0</v>
       </c>
-      <c r="N5" s="457"/>
-      <c r="O5" s="458"/>
+      <c r="N5" s="486"/>
+      <c r="O5" s="487"/>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="290" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="467"/>
+      <c r="B6" s="498"/>
       <c r="C6" s="291" t="s">
         <v>69</v>
       </c>
@@ -4106,7 +4106,7 @@
       <c r="H6" s="293" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="469"/>
+      <c r="I6" s="489"/>
       <c r="J6" s="291" t="s">
         <v>69</v>
       </c>
@@ -4127,20 +4127,20 @@
       <c r="A7" s="294" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="463"/>
-      <c r="C7" s="464"/>
-      <c r="D7" s="464"/>
-      <c r="E7" s="464"/>
-      <c r="F7" s="464"/>
-      <c r="G7" s="464"/>
-      <c r="H7" s="465"/>
-      <c r="I7" s="463"/>
-      <c r="J7" s="464"/>
-      <c r="K7" s="464"/>
-      <c r="L7" s="464"/>
-      <c r="M7" s="464"/>
-      <c r="N7" s="464"/>
-      <c r="O7" s="465"/>
+      <c r="B7" s="453"/>
+      <c r="C7" s="454"/>
+      <c r="D7" s="454"/>
+      <c r="E7" s="454"/>
+      <c r="F7" s="454"/>
+      <c r="G7" s="454"/>
+      <c r="H7" s="455"/>
+      <c r="I7" s="453"/>
+      <c r="J7" s="454"/>
+      <c r="K7" s="454"/>
+      <c r="L7" s="454"/>
+      <c r="M7" s="454"/>
+      <c r="N7" s="454"/>
+      <c r="O7" s="455"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -4339,24 +4339,24 @@
       <c r="A12" s="294" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="463" t="s">
+      <c r="B12" s="453" t="s">
         <v>190</v>
       </c>
-      <c r="C12" s="464"/>
-      <c r="D12" s="464"/>
-      <c r="E12" s="464"/>
-      <c r="F12" s="464"/>
-      <c r="G12" s="464"/>
-      <c r="H12" s="465"/>
-      <c r="I12" s="463" t="s">
+      <c r="C12" s="454"/>
+      <c r="D12" s="454"/>
+      <c r="E12" s="454"/>
+      <c r="F12" s="454"/>
+      <c r="G12" s="454"/>
+      <c r="H12" s="455"/>
+      <c r="I12" s="453" t="s">
         <v>137</v>
       </c>
-      <c r="J12" s="464"/>
-      <c r="K12" s="464"/>
-      <c r="L12" s="464"/>
-      <c r="M12" s="464"/>
-      <c r="N12" s="464"/>
-      <c r="O12" s="465"/>
+      <c r="J12" s="454"/>
+      <c r="K12" s="454"/>
+      <c r="L12" s="454"/>
+      <c r="M12" s="454"/>
+      <c r="N12" s="454"/>
+      <c r="O12" s="455"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -4411,24 +4411,24 @@
       <c r="A14" s="294" t="s">
         <v>139</v>
       </c>
-      <c r="B14" s="463" t="s">
+      <c r="B14" s="453" t="s">
         <v>138</v>
       </c>
-      <c r="C14" s="464"/>
-      <c r="D14" s="464"/>
-      <c r="E14" s="464"/>
-      <c r="F14" s="464"/>
-      <c r="G14" s="464"/>
-      <c r="H14" s="465"/>
-      <c r="I14" s="463" t="s">
-        <v>1</v>
-      </c>
-      <c r="J14" s="464"/>
-      <c r="K14" s="464"/>
-      <c r="L14" s="464"/>
-      <c r="M14" s="464"/>
-      <c r="N14" s="464"/>
-      <c r="O14" s="465"/>
+      <c r="C14" s="454"/>
+      <c r="D14" s="454"/>
+      <c r="E14" s="454"/>
+      <c r="F14" s="454"/>
+      <c r="G14" s="454"/>
+      <c r="H14" s="455"/>
+      <c r="I14" s="453" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="454"/>
+      <c r="K14" s="454"/>
+      <c r="L14" s="454"/>
+      <c r="M14" s="454"/>
+      <c r="N14" s="454"/>
+      <c r="O14" s="455"/>
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -4531,24 +4531,24 @@
       <c r="A17" s="294" t="s">
         <v>191</v>
       </c>
-      <c r="B17" s="463" t="s">
+      <c r="B17" s="453" t="s">
         <v>138</v>
       </c>
-      <c r="C17" s="464"/>
-      <c r="D17" s="464"/>
-      <c r="E17" s="464"/>
-      <c r="F17" s="464"/>
-      <c r="G17" s="464"/>
-      <c r="H17" s="465"/>
-      <c r="I17" s="463" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" s="464"/>
-      <c r="K17" s="464"/>
-      <c r="L17" s="464"/>
-      <c r="M17" s="464"/>
-      <c r="N17" s="464"/>
-      <c r="O17" s="465"/>
+      <c r="C17" s="454"/>
+      <c r="D17" s="454"/>
+      <c r="E17" s="454"/>
+      <c r="F17" s="454"/>
+      <c r="G17" s="454"/>
+      <c r="H17" s="455"/>
+      <c r="I17" s="453" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="454"/>
+      <c r="K17" s="454"/>
+      <c r="L17" s="454"/>
+      <c r="M17" s="454"/>
+      <c r="N17" s="454"/>
+      <c r="O17" s="455"/>
       <c r="P17" s="1"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -4795,25 +4795,25 @@
       <c r="A23" s="300" t="s">
         <v>249</v>
       </c>
-      <c r="B23" s="488">
+      <c r="B23" s="456">
         <v>784</v>
       </c>
-      <c r="C23" s="491">
+      <c r="C23" s="459">
         <v>603</v>
       </c>
-      <c r="D23" s="488">
+      <c r="D23" s="456">
         <v>835</v>
       </c>
-      <c r="E23" s="496">
+      <c r="E23" s="464">
         <v>1080</v>
       </c>
-      <c r="F23" s="491">
+      <c r="F23" s="459">
         <v>267</v>
       </c>
-      <c r="G23" s="488">
+      <c r="G23" s="456">
         <v>673</v>
       </c>
-      <c r="H23" s="496">
+      <c r="H23" s="464">
         <v>1030</v>
       </c>
       <c r="I23" s="301"/>
@@ -4829,13 +4829,13 @@
       <c r="A24" s="304" t="s">
         <v>142</v>
       </c>
-      <c r="B24" s="489"/>
-      <c r="C24" s="492"/>
-      <c r="D24" s="494"/>
-      <c r="E24" s="497"/>
-      <c r="F24" s="492"/>
-      <c r="G24" s="494"/>
-      <c r="H24" s="497"/>
+      <c r="B24" s="457"/>
+      <c r="C24" s="460"/>
+      <c r="D24" s="462"/>
+      <c r="E24" s="465"/>
+      <c r="F24" s="460"/>
+      <c r="G24" s="462"/>
+      <c r="H24" s="465"/>
       <c r="I24" s="305">
         <v>2.6526903390105896</v>
       </c>
@@ -4863,13 +4863,13 @@
       <c r="A25" s="304" t="s">
         <v>143</v>
       </c>
-      <c r="B25" s="489"/>
-      <c r="C25" s="492"/>
-      <c r="D25" s="494"/>
-      <c r="E25" s="497"/>
-      <c r="F25" s="492"/>
-      <c r="G25" s="494"/>
-      <c r="H25" s="497"/>
+      <c r="B25" s="457"/>
+      <c r="C25" s="460"/>
+      <c r="D25" s="462"/>
+      <c r="E25" s="465"/>
+      <c r="F25" s="460"/>
+      <c r="G25" s="462"/>
+      <c r="H25" s="465"/>
       <c r="I25" s="308">
         <v>2.3779694578808535</v>
       </c>
@@ -4897,13 +4897,13 @@
       <c r="A26" s="304" t="s">
         <v>144</v>
       </c>
-      <c r="B26" s="489"/>
-      <c r="C26" s="492"/>
-      <c r="D26" s="494"/>
-      <c r="E26" s="497"/>
-      <c r="F26" s="492"/>
-      <c r="G26" s="494"/>
-      <c r="H26" s="497"/>
+      <c r="B26" s="457"/>
+      <c r="C26" s="460"/>
+      <c r="D26" s="462"/>
+      <c r="E26" s="465"/>
+      <c r="F26" s="460"/>
+      <c r="G26" s="462"/>
+      <c r="H26" s="465"/>
       <c r="I26" s="308">
         <v>2.1666666666666665</v>
       </c>
@@ -4931,13 +4931,13 @@
       <c r="A27" s="311" t="s">
         <v>145</v>
       </c>
-      <c r="B27" s="490"/>
-      <c r="C27" s="493"/>
-      <c r="D27" s="495"/>
-      <c r="E27" s="498"/>
-      <c r="F27" s="493"/>
-      <c r="G27" s="495"/>
-      <c r="H27" s="498"/>
+      <c r="B27" s="458"/>
+      <c r="C27" s="461"/>
+      <c r="D27" s="463"/>
+      <c r="E27" s="466"/>
+      <c r="F27" s="461"/>
+      <c r="G27" s="463"/>
+      <c r="H27" s="466"/>
       <c r="I27" s="312">
         <v>1.9768086876483704</v>
       </c>
@@ -5397,24 +5397,24 @@
       <c r="A37" s="294" t="s">
         <v>262</v>
       </c>
-      <c r="B37" s="463" t="s">
+      <c r="B37" s="453" t="s">
         <v>138</v>
       </c>
-      <c r="C37" s="464"/>
-      <c r="D37" s="464"/>
-      <c r="E37" s="464"/>
-      <c r="F37" s="464"/>
-      <c r="G37" s="464"/>
-      <c r="H37" s="465"/>
-      <c r="I37" s="463" t="s">
-        <v>1</v>
-      </c>
-      <c r="J37" s="464"/>
-      <c r="K37" s="464"/>
-      <c r="L37" s="464"/>
-      <c r="M37" s="464"/>
-      <c r="N37" s="464"/>
-      <c r="O37" s="465"/>
+      <c r="C37" s="454"/>
+      <c r="D37" s="454"/>
+      <c r="E37" s="454"/>
+      <c r="F37" s="454"/>
+      <c r="G37" s="454"/>
+      <c r="H37" s="455"/>
+      <c r="I37" s="453" t="s">
+        <v>1</v>
+      </c>
+      <c r="J37" s="454"/>
+      <c r="K37" s="454"/>
+      <c r="L37" s="454"/>
+      <c r="M37" s="454"/>
+      <c r="N37" s="454"/>
+      <c r="O37" s="455"/>
       <c r="P37" s="1"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -5709,24 +5709,24 @@
       <c r="A44" s="294" t="s">
         <v>154</v>
       </c>
-      <c r="B44" s="463" t="s">
+      <c r="B44" s="453" t="s">
         <v>138</v>
       </c>
-      <c r="C44" s="464"/>
-      <c r="D44" s="464"/>
-      <c r="E44" s="464"/>
-      <c r="F44" s="464"/>
-      <c r="G44" s="464"/>
-      <c r="H44" s="465"/>
-      <c r="I44" s="463" t="s">
-        <v>1</v>
-      </c>
-      <c r="J44" s="464"/>
-      <c r="K44" s="464"/>
-      <c r="L44" s="464"/>
-      <c r="M44" s="464"/>
-      <c r="N44" s="464"/>
-      <c r="O44" s="465"/>
+      <c r="C44" s="454"/>
+      <c r="D44" s="454"/>
+      <c r="E44" s="454"/>
+      <c r="F44" s="454"/>
+      <c r="G44" s="454"/>
+      <c r="H44" s="455"/>
+      <c r="I44" s="453" t="s">
+        <v>1</v>
+      </c>
+      <c r="J44" s="454"/>
+      <c r="K44" s="454"/>
+      <c r="L44" s="454"/>
+      <c r="M44" s="454"/>
+      <c r="N44" s="454"/>
+      <c r="O44" s="455"/>
       <c r="P44" s="1"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -5860,45 +5860,45 @@
       <c r="O48"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" s="461" t="s">
+      <c r="A49" s="495" t="s">
         <v>192</v>
       </c>
-      <c r="B49" s="462"/>
-      <c r="C49" s="462"/>
-      <c r="D49" s="462"/>
-      <c r="E49" s="462"/>
-      <c r="F49" s="462"/>
-      <c r="G49" s="462"/>
-      <c r="H49" s="462"/>
-      <c r="I49" s="462"/>
-      <c r="J49" s="462"/>
-      <c r="K49" s="462"/>
-      <c r="L49" s="462"/>
-      <c r="M49" s="462"/>
-      <c r="N49" s="462"/>
-      <c r="O49" s="462"/>
+      <c r="B49" s="496"/>
+      <c r="C49" s="496"/>
+      <c r="D49" s="496"/>
+      <c r="E49" s="496"/>
+      <c r="F49" s="496"/>
+      <c r="G49" s="496"/>
+      <c r="H49" s="496"/>
+      <c r="I49" s="496"/>
+      <c r="J49" s="496"/>
+      <c r="K49" s="496"/>
+      <c r="L49" s="496"/>
+      <c r="M49" s="496"/>
+      <c r="N49" s="496"/>
+      <c r="O49" s="496"/>
       <c r="P49" s="1"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="418"/>
-      <c r="B50" s="459" t="s">
+      <c r="B50" s="485" t="s">
         <v>130</v>
       </c>
-      <c r="C50" s="457"/>
-      <c r="D50" s="457"/>
-      <c r="E50" s="457"/>
-      <c r="F50" s="457"/>
-      <c r="G50" s="457"/>
-      <c r="H50" s="458"/>
-      <c r="I50" s="459" t="s">
+      <c r="C50" s="486"/>
+      <c r="D50" s="486"/>
+      <c r="E50" s="486"/>
+      <c r="F50" s="486"/>
+      <c r="G50" s="486"/>
+      <c r="H50" s="487"/>
+      <c r="I50" s="485" t="s">
         <v>131</v>
       </c>
-      <c r="J50" s="457"/>
-      <c r="K50" s="457"/>
-      <c r="L50" s="457"/>
-      <c r="M50" s="457"/>
-      <c r="N50" s="457"/>
-      <c r="O50" s="458"/>
+      <c r="J50" s="486"/>
+      <c r="K50" s="486"/>
+      <c r="L50" s="486"/>
+      <c r="M50" s="486"/>
+      <c r="N50" s="486"/>
+      <c r="O50" s="487"/>
       <c r="P50" s="1"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -5906,29 +5906,29 @@
       <c r="B51" s="420" t="s">
         <v>67</v>
       </c>
-      <c r="C51" s="459">
+      <c r="C51" s="485">
         <v>2030</v>
       </c>
-      <c r="D51" s="457"/>
-      <c r="E51" s="458"/>
-      <c r="F51" s="459" t="s">
+      <c r="D51" s="486"/>
+      <c r="E51" s="487"/>
+      <c r="F51" s="485" t="s">
         <v>0</v>
       </c>
-      <c r="G51" s="457"/>
-      <c r="H51" s="458"/>
+      <c r="G51" s="486"/>
+      <c r="H51" s="487"/>
       <c r="I51" s="420" t="s">
         <v>67</v>
       </c>
-      <c r="J51" s="459">
+      <c r="J51" s="485">
         <v>2030</v>
       </c>
-      <c r="K51" s="457"/>
-      <c r="L51" s="458"/>
-      <c r="M51" s="459" t="s">
+      <c r="K51" s="486"/>
+      <c r="L51" s="487"/>
+      <c r="M51" s="485" t="s">
         <v>0</v>
       </c>
-      <c r="N51" s="457"/>
-      <c r="O51" s="458"/>
+      <c r="N51" s="486"/>
+      <c r="O51" s="487"/>
       <c r="P51" s="1"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -5971,24 +5971,24 @@
       <c r="A53" s="315" t="s">
         <v>193</v>
       </c>
-      <c r="B53" s="470" t="s">
+      <c r="B53" s="467" t="s">
         <v>57</v>
       </c>
-      <c r="C53" s="471"/>
-      <c r="D53" s="471"/>
-      <c r="E53" s="471"/>
-      <c r="F53" s="471"/>
-      <c r="G53" s="471"/>
-      <c r="H53" s="472"/>
-      <c r="I53" s="473" t="s">
+      <c r="C53" s="468"/>
+      <c r="D53" s="468"/>
+      <c r="E53" s="468"/>
+      <c r="F53" s="468"/>
+      <c r="G53" s="468"/>
+      <c r="H53" s="469"/>
+      <c r="I53" s="470" t="s">
         <v>132</v>
       </c>
-      <c r="J53" s="474"/>
-      <c r="K53" s="474"/>
-      <c r="L53" s="474"/>
-      <c r="M53" s="474"/>
-      <c r="N53" s="474"/>
-      <c r="O53" s="475"/>
+      <c r="J53" s="471"/>
+      <c r="K53" s="471"/>
+      <c r="L53" s="471"/>
+      <c r="M53" s="471"/>
+      <c r="N53" s="471"/>
+      <c r="O53" s="472"/>
       <c r="P53" s="1"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -6043,24 +6043,24 @@
       <c r="A55" s="315" t="s">
         <v>191</v>
       </c>
-      <c r="B55" s="470" t="s">
+      <c r="B55" s="467" t="s">
         <v>138</v>
       </c>
-      <c r="C55" s="471"/>
-      <c r="D55" s="471"/>
-      <c r="E55" s="471"/>
-      <c r="F55" s="471"/>
-      <c r="G55" s="471"/>
-      <c r="H55" s="472"/>
-      <c r="I55" s="470" t="s">
-        <v>1</v>
-      </c>
-      <c r="J55" s="471"/>
-      <c r="K55" s="471"/>
-      <c r="L55" s="471"/>
-      <c r="M55" s="471"/>
-      <c r="N55" s="471"/>
-      <c r="O55" s="472"/>
+      <c r="C55" s="468"/>
+      <c r="D55" s="468"/>
+      <c r="E55" s="468"/>
+      <c r="F55" s="468"/>
+      <c r="G55" s="468"/>
+      <c r="H55" s="469"/>
+      <c r="I55" s="467" t="s">
+        <v>1</v>
+      </c>
+      <c r="J55" s="468"/>
+      <c r="K55" s="468"/>
+      <c r="L55" s="468"/>
+      <c r="M55" s="468"/>
+      <c r="N55" s="468"/>
+      <c r="O55" s="469"/>
       <c r="P55" s="1"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -6163,25 +6163,25 @@
       <c r="A58" s="46" t="s">
         <v>249</v>
       </c>
-      <c r="B58" s="476">
+      <c r="B58" s="473">
         <v>548.72999999999979</v>
       </c>
-      <c r="C58" s="479">
+      <c r="C58" s="476">
         <v>421.97336999999987</v>
       </c>
-      <c r="D58" s="482">
+      <c r="D58" s="479">
         <v>584.5</v>
       </c>
-      <c r="E58" s="485">
+      <c r="E58" s="482">
         <v>756</v>
       </c>
-      <c r="F58" s="479">
+      <c r="F58" s="476">
         <v>186.56819999999993</v>
       </c>
-      <c r="G58" s="482">
+      <c r="G58" s="479">
         <v>470.74999999999989</v>
       </c>
-      <c r="H58" s="485">
+      <c r="H58" s="482">
         <v>669.36187499999994</v>
       </c>
       <c r="I58" s="301"/>
@@ -6197,13 +6197,13 @@
       <c r="A59" s="61" t="s">
         <v>263</v>
       </c>
-      <c r="B59" s="477"/>
-      <c r="C59" s="480"/>
-      <c r="D59" s="483"/>
-      <c r="E59" s="486"/>
-      <c r="F59" s="480"/>
-      <c r="G59" s="483"/>
-      <c r="H59" s="486"/>
+      <c r="B59" s="474"/>
+      <c r="C59" s="477"/>
+      <c r="D59" s="480"/>
+      <c r="E59" s="483"/>
+      <c r="F59" s="477"/>
+      <c r="G59" s="480"/>
+      <c r="H59" s="483"/>
       <c r="I59" s="67">
         <v>2.6526903390105896</v>
       </c>
@@ -6231,13 +6231,13 @@
       <c r="A60" s="61" t="s">
         <v>143</v>
       </c>
-      <c r="B60" s="477"/>
-      <c r="C60" s="480"/>
-      <c r="D60" s="483"/>
-      <c r="E60" s="486"/>
-      <c r="F60" s="480"/>
-      <c r="G60" s="483"/>
-      <c r="H60" s="486"/>
+      <c r="B60" s="474"/>
+      <c r="C60" s="477"/>
+      <c r="D60" s="480"/>
+      <c r="E60" s="483"/>
+      <c r="F60" s="477"/>
+      <c r="G60" s="480"/>
+      <c r="H60" s="483"/>
       <c r="I60" s="67">
         <v>2.3779694578808535</v>
       </c>
@@ -6265,13 +6265,13 @@
       <c r="A61" s="61" t="s">
         <v>144</v>
       </c>
-      <c r="B61" s="477"/>
-      <c r="C61" s="480"/>
-      <c r="D61" s="483"/>
-      <c r="E61" s="486"/>
-      <c r="F61" s="480"/>
-      <c r="G61" s="483"/>
-      <c r="H61" s="486"/>
+      <c r="B61" s="474"/>
+      <c r="C61" s="477"/>
+      <c r="D61" s="480"/>
+      <c r="E61" s="483"/>
+      <c r="F61" s="477"/>
+      <c r="G61" s="480"/>
+      <c r="H61" s="483"/>
       <c r="I61" s="67">
         <v>2.1666666666666665</v>
       </c>
@@ -6299,13 +6299,13 @@
       <c r="A62" s="61" t="s">
         <v>145</v>
       </c>
-      <c r="B62" s="478"/>
-      <c r="C62" s="481"/>
-      <c r="D62" s="484"/>
-      <c r="E62" s="487"/>
-      <c r="F62" s="481"/>
-      <c r="G62" s="484"/>
-      <c r="H62" s="487"/>
+      <c r="B62" s="475"/>
+      <c r="C62" s="478"/>
+      <c r="D62" s="481"/>
+      <c r="E62" s="484"/>
+      <c r="F62" s="478"/>
+      <c r="G62" s="481"/>
+      <c r="H62" s="484"/>
       <c r="I62" s="67">
         <v>1.9768086876483704</v>
       </c>
@@ -6477,24 +6477,24 @@
       <c r="A66" s="315" t="s">
         <v>194</v>
       </c>
-      <c r="B66" s="470" t="s">
+      <c r="B66" s="467" t="s">
         <v>138</v>
       </c>
-      <c r="C66" s="471"/>
-      <c r="D66" s="471"/>
-      <c r="E66" s="471"/>
-      <c r="F66" s="471"/>
-      <c r="G66" s="471"/>
-      <c r="H66" s="472"/>
-      <c r="I66" s="470" t="s">
-        <v>1</v>
-      </c>
-      <c r="J66" s="471"/>
-      <c r="K66" s="471"/>
-      <c r="L66" s="471"/>
-      <c r="M66" s="471"/>
-      <c r="N66" s="471"/>
-      <c r="O66" s="472"/>
+      <c r="C66" s="468"/>
+      <c r="D66" s="468"/>
+      <c r="E66" s="468"/>
+      <c r="F66" s="468"/>
+      <c r="G66" s="468"/>
+      <c r="H66" s="469"/>
+      <c r="I66" s="467" t="s">
+        <v>1</v>
+      </c>
+      <c r="J66" s="468"/>
+      <c r="K66" s="468"/>
+      <c r="L66" s="468"/>
+      <c r="M66" s="468"/>
+      <c r="N66" s="468"/>
+      <c r="O66" s="469"/>
       <c r="P66" s="1"/>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
@@ -6647,17 +6647,17 @@
       </c>
     </row>
     <row r="72" spans="1:16" ht="294.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="460" t="s">
+      <c r="A72" s="494" t="s">
         <v>156</v>
       </c>
-      <c r="B72" s="460"/>
-      <c r="C72" s="460"/>
-      <c r="D72" s="460"/>
-      <c r="E72" s="460"/>
-      <c r="F72" s="460"/>
-      <c r="G72" s="460"/>
-      <c r="H72" s="460"/>
-      <c r="I72" s="460"/>
+      <c r="B72" s="494"/>
+      <c r="C72" s="494"/>
+      <c r="D72" s="494"/>
+      <c r="E72" s="494"/>
+      <c r="F72" s="494"/>
+      <c r="G72" s="494"/>
+      <c r="H72" s="494"/>
+      <c r="I72" s="494"/>
       <c r="J72" s="45"/>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
@@ -6672,40 +6672,6 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="I14:O14"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="E23:E27"/>
-    <mergeCell ref="F23:F27"/>
-    <mergeCell ref="G23:G27"/>
-    <mergeCell ref="H23:H27"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B66:H66"/>
-    <mergeCell ref="I66:O66"/>
-    <mergeCell ref="B53:H53"/>
-    <mergeCell ref="I53:O53"/>
-    <mergeCell ref="B55:H55"/>
-    <mergeCell ref="I55:O55"/>
-    <mergeCell ref="B58:B62"/>
-    <mergeCell ref="C58:C62"/>
-    <mergeCell ref="D58:D62"/>
-    <mergeCell ref="E58:E62"/>
-    <mergeCell ref="F58:F62"/>
-    <mergeCell ref="G58:G62"/>
-    <mergeCell ref="H58:H62"/>
-    <mergeCell ref="I37:O37"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="I44:O44"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="I17:O17"/>
-    <mergeCell ref="B37:H37"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="I7:O7"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="A3:O3"/>
     <mergeCell ref="B4:H4"/>
@@ -6722,6 +6688,40 @@
     <mergeCell ref="I12:O12"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="I7:O7"/>
+    <mergeCell ref="I37:O37"/>
+    <mergeCell ref="B44:H44"/>
+    <mergeCell ref="I44:O44"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="I17:O17"/>
+    <mergeCell ref="B37:H37"/>
+    <mergeCell ref="B66:H66"/>
+    <mergeCell ref="I66:O66"/>
+    <mergeCell ref="B53:H53"/>
+    <mergeCell ref="I53:O53"/>
+    <mergeCell ref="B55:H55"/>
+    <mergeCell ref="I55:O55"/>
+    <mergeCell ref="B58:B62"/>
+    <mergeCell ref="C58:C62"/>
+    <mergeCell ref="D58:D62"/>
+    <mergeCell ref="E58:E62"/>
+    <mergeCell ref="F58:F62"/>
+    <mergeCell ref="G58:G62"/>
+    <mergeCell ref="H58:H62"/>
+    <mergeCell ref="I14:O14"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="E23:E27"/>
+    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="G23:G27"/>
+    <mergeCell ref="H23:H27"/>
+    <mergeCell ref="B14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6750,13 +6750,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="453" t="s">
+      <c r="A1" s="490" t="s">
         <v>316</v>
       </c>
-      <c r="B1" s="454"/>
-      <c r="C1" s="454"/>
-      <c r="D1" s="454"/>
-      <c r="E1" s="454"/>
+      <c r="B1" s="491"/>
+      <c r="C1" s="491"/>
+      <c r="D1" s="491"/>
+      <c r="E1" s="491"/>
     </row>
     <row r="2" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:14" ht="37.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7587,13 +7587,13 @@
       <c r="N37" s="1"/>
     </row>
     <row r="38" spans="1:14" ht="91.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="460" t="s">
+      <c r="A38" s="494" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="460"/>
-      <c r="C38" s="460"/>
-      <c r="D38" s="460"/>
-      <c r="E38" s="460"/>
+      <c r="B38" s="494"/>
+      <c r="C38" s="494"/>
+      <c r="D38" s="494"/>
+      <c r="E38" s="494"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -12261,12 +12261,12 @@
   </sheetPr>
   <dimension ref="A1:AU80"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection activeCell="I8" sqref="I8"/>
       <selection pane="topRight" activeCell="I8" sqref="I8"/>
       <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
-      <selection pane="bottomRight" activeCell="J36" sqref="J36"/>
+      <selection pane="bottomRight" activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12321,36 +12321,36 @@
     </row>
     <row r="2" spans="1:47" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="316"/>
-      <c r="B2" s="525" t="s">
+      <c r="B2" s="521" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="526"/>
-      <c r="D2" s="526"/>
-      <c r="E2" s="526"/>
-      <c r="F2" s="526" t="s">
+      <c r="C2" s="522"/>
+      <c r="D2" s="522"/>
+      <c r="E2" s="522"/>
+      <c r="F2" s="522" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="526"/>
-      <c r="H2" s="526"/>
-      <c r="I2" s="526"/>
-      <c r="J2" s="526" t="s">
+      <c r="G2" s="522"/>
+      <c r="H2" s="522"/>
+      <c r="I2" s="522"/>
+      <c r="J2" s="522" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="526"/>
-      <c r="L2" s="526"/>
-      <c r="M2" s="526"/>
-      <c r="N2" s="526" t="s">
+      <c r="K2" s="522"/>
+      <c r="L2" s="522"/>
+      <c r="M2" s="522"/>
+      <c r="N2" s="522" t="s">
         <v>64</v>
       </c>
-      <c r="O2" s="526"/>
-      <c r="P2" s="526"/>
-      <c r="Q2" s="526"/>
-      <c r="R2" s="526" t="s">
+      <c r="O2" s="522"/>
+      <c r="P2" s="522"/>
+      <c r="Q2" s="522"/>
+      <c r="R2" s="522" t="s">
         <v>61</v>
       </c>
-      <c r="S2" s="526"/>
-      <c r="T2" s="526"/>
-      <c r="U2" s="526"/>
+      <c r="S2" s="522"/>
+      <c r="T2" s="522"/>
+      <c r="U2" s="522"/>
       <c r="V2" s="322" t="s">
         <v>314</v>
       </c>
@@ -12360,36 +12360,36 @@
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="317"/>
-      <c r="B3" s="523" t="s">
+      <c r="B3" s="526" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="524"/>
-      <c r="D3" s="524"/>
-      <c r="E3" s="524"/>
-      <c r="F3" s="524" t="s">
+      <c r="C3" s="520"/>
+      <c r="D3" s="520"/>
+      <c r="E3" s="520"/>
+      <c r="F3" s="520" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="524"/>
-      <c r="H3" s="524"/>
-      <c r="I3" s="524"/>
-      <c r="J3" s="524" t="s">
+      <c r="G3" s="520"/>
+      <c r="H3" s="520"/>
+      <c r="I3" s="520"/>
+      <c r="J3" s="520" t="s">
         <v>58</v>
       </c>
-      <c r="K3" s="524"/>
-      <c r="L3" s="524"/>
-      <c r="M3" s="524"/>
-      <c r="N3" s="524" t="s">
+      <c r="K3" s="520"/>
+      <c r="L3" s="520"/>
+      <c r="M3" s="520"/>
+      <c r="N3" s="520" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="524"/>
-      <c r="P3" s="524"/>
-      <c r="Q3" s="524"/>
-      <c r="R3" s="524" t="s">
-        <v>1</v>
-      </c>
-      <c r="S3" s="524"/>
-      <c r="T3" s="524"/>
-      <c r="U3" s="524"/>
+      <c r="O3" s="520"/>
+      <c r="P3" s="520"/>
+      <c r="Q3" s="520"/>
+      <c r="R3" s="520" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="520"/>
+      <c r="T3" s="520"/>
+      <c r="U3" s="520"/>
       <c r="V3" s="322" t="s">
         <v>20</v>
       </c>
@@ -14316,12 +14316,12 @@
       <c r="A31" s="387" t="s">
         <v>164</v>
       </c>
-      <c r="B31" s="520" t="s">
+      <c r="B31" s="523" t="s">
         <v>165</v>
       </c>
-      <c r="C31" s="521"/>
-      <c r="D31" s="521"/>
-      <c r="E31" s="522"/>
+      <c r="C31" s="524"/>
+      <c r="D31" s="524"/>
+      <c r="E31" s="525"/>
       <c r="F31" s="413"/>
       <c r="G31" s="413"/>
       <c r="H31" s="413"/>
@@ -17395,17 +17395,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
     <mergeCell ref="R3:U3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:U2"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:Q3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -17419,9 +17419,9 @@
   </sheetPr>
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17460,34 +17460,34 @@
       <c r="O1" s="511"/>
     </row>
     <row r="3" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="527" t="s">
+      <c r="A3" s="528" t="s">
         <v>168</v>
       </c>
-      <c r="B3" s="529" t="s">
+      <c r="B3" s="530" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="529"/>
-      <c r="D3" s="529"/>
-      <c r="E3" s="530" t="s">
+      <c r="C3" s="530"/>
+      <c r="D3" s="530"/>
+      <c r="E3" s="531" t="s">
         <v>295</v>
       </c>
-      <c r="F3" s="529"/>
-      <c r="G3" s="531"/>
-      <c r="H3" s="529" t="s">
+      <c r="F3" s="530"/>
+      <c r="G3" s="532"/>
+      <c r="H3" s="530" t="s">
         <v>169</v>
       </c>
-      <c r="I3" s="529"/>
-      <c r="J3" s="529"/>
-      <c r="K3" s="529"/>
-      <c r="L3" s="529"/>
-      <c r="M3" s="529"/>
-      <c r="N3" s="530" t="s">
+      <c r="I3" s="530"/>
+      <c r="J3" s="530"/>
+      <c r="K3" s="530"/>
+      <c r="L3" s="530"/>
+      <c r="M3" s="530"/>
+      <c r="N3" s="531" t="s">
         <v>170</v>
       </c>
-      <c r="O3" s="532"/>
+      <c r="O3" s="533"/>
     </row>
     <row r="4" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="528"/>
+      <c r="A4" s="529"/>
       <c r="B4" s="84">
         <v>2020</v>
       </c>
@@ -18409,30 +18409,30 @@
       <c r="M26" s="196"/>
     </row>
     <row r="27" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="527" t="s">
+      <c r="A27" s="528" t="s">
         <v>184</v>
       </c>
-      <c r="B27" s="529" t="s">
+      <c r="B27" s="530" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="529"/>
-      <c r="D27" s="529"/>
-      <c r="E27" s="530" t="s">
+      <c r="C27" s="530"/>
+      <c r="D27" s="530"/>
+      <c r="E27" s="531" t="s">
         <v>296</v>
       </c>
-      <c r="F27" s="529"/>
-      <c r="G27" s="531"/>
-      <c r="H27" s="529" t="s">
+      <c r="F27" s="530"/>
+      <c r="G27" s="532"/>
+      <c r="H27" s="530" t="s">
         <v>41</v>
       </c>
-      <c r="I27" s="529"/>
-      <c r="J27" s="532"/>
+      <c r="I27" s="530"/>
+      <c r="J27" s="533"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="528"/>
+      <c r="A28" s="529"/>
       <c r="B28" s="84">
         <v>2015</v>
       </c>
@@ -18606,21 +18606,21 @@
     </row>
     <row r="33" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="213"/>
-      <c r="B33" s="529" t="s">
+      <c r="B33" s="530" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="529"/>
-      <c r="D33" s="529"/>
-      <c r="E33" s="530" t="s">
+      <c r="C33" s="530"/>
+      <c r="D33" s="530"/>
+      <c r="E33" s="531" t="s">
         <v>297</v>
       </c>
-      <c r="F33" s="529"/>
-      <c r="G33" s="531"/>
-      <c r="H33" s="529" t="s">
+      <c r="F33" s="530"/>
+      <c r="G33" s="532"/>
+      <c r="H33" s="530" t="s">
         <v>45</v>
       </c>
-      <c r="I33" s="529"/>
-      <c r="J33" s="532"/>
+      <c r="I33" s="530"/>
+      <c r="J33" s="533"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
@@ -18695,21 +18695,21 @@
     </row>
     <row r="36" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="219"/>
-      <c r="B36" s="529" t="s">
+      <c r="B36" s="530" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="529"/>
-      <c r="D36" s="529"/>
-      <c r="E36" s="530" t="s">
+      <c r="C36" s="530"/>
+      <c r="D36" s="530"/>
+      <c r="E36" s="531" t="s">
         <v>296</v>
       </c>
-      <c r="F36" s="529"/>
-      <c r="G36" s="531"/>
-      <c r="H36" s="529" t="s">
+      <c r="F36" s="530"/>
+      <c r="G36" s="532"/>
+      <c r="H36" s="530" t="s">
         <v>45</v>
       </c>
-      <c r="I36" s="529"/>
-      <c r="J36" s="532"/>
+      <c r="I36" s="530"/>
+      <c r="J36" s="533"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
@@ -18863,32 +18863,32 @@
       <c r="M42" s="2"/>
     </row>
     <row r="43" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="527" t="s">
+      <c r="A43" s="528" t="s">
         <v>185</v>
       </c>
-      <c r="B43" s="529" t="s">
+      <c r="B43" s="530" t="s">
         <v>300</v>
       </c>
-      <c r="C43" s="529"/>
-      <c r="D43" s="529"/>
-      <c r="E43" s="530" t="s">
+      <c r="C43" s="530"/>
+      <c r="D43" s="530"/>
+      <c r="E43" s="531" t="s">
         <v>298</v>
       </c>
-      <c r="F43" s="529"/>
-      <c r="G43" s="531"/>
-      <c r="H43" s="529" t="s">
+      <c r="F43" s="530"/>
+      <c r="G43" s="532"/>
+      <c r="H43" s="530" t="s">
         <v>46</v>
       </c>
-      <c r="I43" s="529"/>
-      <c r="J43" s="529"/>
-      <c r="K43" s="530" t="s">
+      <c r="I43" s="530"/>
+      <c r="J43" s="530"/>
+      <c r="K43" s="531" t="s">
         <v>186</v>
       </c>
-      <c r="L43" s="529"/>
-      <c r="M43" s="532"/>
+      <c r="L43" s="530"/>
+      <c r="M43" s="533"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="528"/>
+      <c r="A44" s="529"/>
       <c r="B44" s="84">
         <v>2020</v>
       </c>
@@ -19539,57 +19539,73 @@
       <c r="M61" s="272"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="533" t="s">
+      <c r="A62" s="527" t="s">
         <v>188</v>
       </c>
-      <c r="B62" s="533"/>
-      <c r="C62" s="533"/>
-      <c r="D62" s="533"/>
-      <c r="E62" s="533"/>
-      <c r="F62" s="533"/>
-      <c r="G62" s="533"/>
-      <c r="H62" s="533"/>
-      <c r="I62" s="533"/>
-      <c r="J62" s="533"/>
-      <c r="K62" s="533"/>
-      <c r="L62" s="533"/>
-      <c r="M62" s="533"/>
+      <c r="B62" s="527"/>
+      <c r="C62" s="527"/>
+      <c r="D62" s="527"/>
+      <c r="E62" s="527"/>
+      <c r="F62" s="527"/>
+      <c r="G62" s="527"/>
+      <c r="H62" s="527"/>
+      <c r="I62" s="527"/>
+      <c r="J62" s="527"/>
+      <c r="K62" s="527"/>
+      <c r="L62" s="527"/>
+      <c r="M62" s="527"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="533"/>
-      <c r="B63" s="533"/>
-      <c r="C63" s="533"/>
-      <c r="D63" s="533"/>
-      <c r="E63" s="533"/>
-      <c r="F63" s="533"/>
-      <c r="G63" s="533"/>
-      <c r="H63" s="533"/>
-      <c r="I63" s="533"/>
-      <c r="J63" s="533"/>
-      <c r="K63" s="533"/>
-      <c r="L63" s="533"/>
-      <c r="M63" s="533"/>
+      <c r="A63" s="527"/>
+      <c r="B63" s="527"/>
+      <c r="C63" s="527"/>
+      <c r="D63" s="527"/>
+      <c r="E63" s="527"/>
+      <c r="F63" s="527"/>
+      <c r="G63" s="527"/>
+      <c r="H63" s="527"/>
+      <c r="I63" s="527"/>
+      <c r="J63" s="527"/>
+      <c r="K63" s="527"/>
+      <c r="L63" s="527"/>
+      <c r="M63" s="527"/>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="533"/>
-      <c r="B64" s="533"/>
-      <c r="C64" s="533"/>
-      <c r="D64" s="533"/>
-      <c r="E64" s="533"/>
-      <c r="F64" s="533"/>
-      <c r="G64" s="533"/>
-      <c r="H64" s="533"/>
-      <c r="I64" s="533"/>
-      <c r="J64" s="533"/>
-      <c r="K64" s="533"/>
-      <c r="L64" s="533"/>
-      <c r="M64" s="533"/>
+      <c r="A64" s="527"/>
+      <c r="B64" s="527"/>
+      <c r="C64" s="527"/>
+      <c r="D64" s="527"/>
+      <c r="E64" s="527"/>
+      <c r="F64" s="527"/>
+      <c r="G64" s="527"/>
+      <c r="H64" s="527"/>
+      <c r="I64" s="527"/>
+      <c r="J64" s="527"/>
+      <c r="K64" s="527"/>
+      <c r="L64" s="527"/>
+      <c r="M64" s="527"/>
     </row>
     <row r="66" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F66" s="273"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:J36"/>
     <mergeCell ref="A62:M64"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:D43"/>
@@ -19600,22 +19616,6 @@
     <mergeCell ref="E57:G57"/>
     <mergeCell ref="H57:J57"/>
     <mergeCell ref="K57:M57"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="H27:J27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>